<commit_message>
add transaction page update
- Update db design
- Update mainpage
- Complete transaction page
</commit_message>
<xml_diff>
--- a/databasedesign.xlsx
+++ b/databasedesign.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maitv_a05383\Documents\GitHub\ProjectSem1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mai\Documents\GitHub\ProjectSem1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="databases" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <t>0-default/1-addnewbyuser</t>
   </si>
   <si>
-    <t>0-loan/1-debt/2-normal</t>
+    <t>0-loan(debt)/1-normal</t>
   </si>
 </sst>
 </file>
@@ -598,22 +598,22 @@
   <dimension ref="C2:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
@@ -622,7 +622,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
@@ -631,7 +631,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
@@ -640,7 +640,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
@@ -649,7 +649,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
@@ -658,8 +658,8 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="9" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
@@ -671,7 +671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" s="6" t="s">
         <v>0</v>
       </c>
@@ -692,7 +692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12" s="6" t="s">
         <v>3</v>
       </c>
@@ -704,7 +704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" s="6" t="s">
         <v>4</v>
       </c>
@@ -718,7 +718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14" s="6" t="s">
         <v>8</v>
       </c>
@@ -732,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="12" t="s">
         <v>27</v>
       </c>
@@ -746,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -754,12 +754,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G17">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>9</v>
       </c>
@@ -771,7 +771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" s="6" t="s">
         <v>10</v>
       </c>
@@ -783,7 +783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C20" s="6" t="s">
         <v>11</v>
       </c>
@@ -795,7 +795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21" s="6" t="s">
         <v>12</v>
       </c>
@@ -804,7 +804,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C22" s="6" t="s">
         <v>0</v>
       </c>
@@ -813,7 +813,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C23" s="6" t="s">
         <v>7</v>
       </c>
@@ -822,7 +822,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C24" s="8" t="s">
         <v>13</v>
       </c>
@@ -831,13 +831,13 @@
       </c>
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
         <v>21</v>
       </c>
@@ -846,7 +846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C28" s="8" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
update mainpage and list transaction page
</commit_message>
<xml_diff>
--- a/databasedesign.xlsx
+++ b/databasedesign.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>CategoryID</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>0-loan(debt)/1-normal</t>
+  </si>
+  <si>
+    <t>isInitialization</t>
+  </si>
+  <si>
+    <t>0- not initialization /1 - initialization</t>
+  </si>
+  <si>
+    <t>If initialization is 1 =&gt; catID = 1</t>
   </si>
 </sst>
 </file>
@@ -151,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -294,11 +303,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -315,6 +363,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,17 +646,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J28"/>
+  <dimension ref="C2:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -678,7 +729,9 @@
       <c r="D11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="G11" t="s">
         <v>0</v>
       </c>
@@ -732,128 +785,139 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="12" t="s">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="G16">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="G17">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G17">
+    <row r="18" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G18">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="3" t="s">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="G19">
-        <v>8</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C20" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E20" s="7"/>
       <c r="G20">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E21" s="7"/>
+      <c r="G21">
+        <v>9</v>
+      </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C22" s="6" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="8" t="s">
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C27" s="3" t="s">
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="3:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="8" t="s">
+    <row r="29" spans="3:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E29" s="11" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>